<commit_message>
Correzione messaggio di errore per timeout
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111#SYSDATSANITASRLXX/SYSDATSANITASRL/SYS-CLINIQUE/6.3.29.3/report-checklist.xlsx
+++ b/GATEWAY/S1#111#SYSDATSANITASRLXX/SYSDATSANITASRL/SYS-CLINIQUE/6.3.29.3/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pelucchis\Documents\repository\it-fse-accreditamento\GATEWAY\S1#111#SYSDATSANITASRLXX\SYSDATSANITASRL\SYS-CLINIQUE\6.3.29.3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3C80911-8097-41C9-BE70-F3739141B608}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8388B3D3-C5DC-4B9D-874C-83F56BC72B9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2003,9 +2003,6 @@
     <t>La diagnosi di accettazione è gestita solo come diagnosi descrittiva, non viene rilevata la codifica ICD9CM</t>
   </si>
   <si>
-    <t>Documento strutturato non valido</t>
-  </si>
-  <si>
     <t>L'operazione deve essere ripetuta</t>
   </si>
   <si>
@@ -2262,6 +2259,9 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.690099.4.4.3416ff7b8ac0722a66aa7fd83f21413eb9b0b7279046c855cba4b79db12595fe.ba9c8df28e^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>Nessuna risposta ricevuta</t>
   </si>
 </sst>
 </file>
@@ -4572,10 +4572,10 @@
   <dimension ref="A1:AA809"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="9" topLeftCell="B10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="9" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="B10" sqref="B10"/>
+      <selection pane="bottomRight" activeCell="O227" sqref="O227"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -4885,13 +4885,13 @@
         <v>45544</v>
       </c>
       <c r="G10" s="33" t="s">
+        <v>588</v>
+      </c>
+      <c r="H10" s="33" t="s">
         <v>589</v>
       </c>
-      <c r="H10" s="33" t="s">
+      <c r="I10" s="33" t="s">
         <v>590</v>
-      </c>
-      <c r="I10" s="33" t="s">
-        <v>591</v>
       </c>
       <c r="J10" s="34" t="s">
         <v>87</v>
@@ -4932,13 +4932,13 @@
         <v>45544</v>
       </c>
       <c r="G11" s="33" t="s">
+        <v>591</v>
+      </c>
+      <c r="H11" s="33" t="s">
         <v>592</v>
       </c>
-      <c r="H11" s="33" t="s">
+      <c r="I11" s="33" t="s">
         <v>593</v>
-      </c>
-      <c r="I11" s="33" t="s">
-        <v>594</v>
       </c>
       <c r="J11" s="34" t="s">
         <v>87</v>
@@ -4996,7 +4996,7 @@
       <c r="T12" s="34"/>
       <c r="U12" s="35"/>
       <c r="V12" s="34" t="s">
-        <v>568</v>
+        <v>567</v>
       </c>
       <c r="W12" s="36" t="s">
         <v>37</v>
@@ -5022,13 +5022,13 @@
         <v>45544</v>
       </c>
       <c r="G13" s="33" t="s">
+        <v>597</v>
+      </c>
+      <c r="H13" s="33" t="s">
         <v>598</v>
       </c>
-      <c r="H13" s="33" t="s">
+      <c r="I13" s="33" t="s">
         <v>599</v>
-      </c>
-      <c r="I13" s="33" t="s">
-        <v>600</v>
       </c>
       <c r="J13" s="34" t="s">
         <v>87</v>
@@ -5069,13 +5069,13 @@
         <v>45544</v>
       </c>
       <c r="G14" s="33" t="s">
+        <v>594</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>596</v>
+      </c>
+      <c r="I14" s="33" t="s">
         <v>595</v>
-      </c>
-      <c r="H14" s="33" t="s">
-        <v>597</v>
-      </c>
-      <c r="I14" s="33" t="s">
-        <v>596</v>
       </c>
       <c r="J14" s="34" t="s">
         <v>87</v>
@@ -6503,7 +6503,7 @@
         <v>87</v>
       </c>
       <c r="O47" s="34" t="s">
-        <v>570</v>
+        <v>606</v>
       </c>
       <c r="P47" s="34" t="s">
         <v>87</v>
@@ -6515,7 +6515,7 @@
         <v>87</v>
       </c>
       <c r="S47" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T47" s="34"/>
       <c r="U47" s="35" t="s">
@@ -6558,7 +6558,7 @@
         <v>87</v>
       </c>
       <c r="O48" s="34" t="s">
-        <v>520</v>
+        <v>606</v>
       </c>
       <c r="P48" s="34" t="s">
         <v>87</v>
@@ -6570,7 +6570,7 @@
         <v>87</v>
       </c>
       <c r="S48" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T48" s="34"/>
       <c r="U48" s="35" t="s">
@@ -6658,7 +6658,7 @@
         <v>87</v>
       </c>
       <c r="O50" s="34" t="s">
-        <v>520</v>
+        <v>606</v>
       </c>
       <c r="P50" s="34" t="s">
         <v>87</v>
@@ -6670,7 +6670,7 @@
         <v>87</v>
       </c>
       <c r="S50" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T50" s="34"/>
       <c r="U50" s="35" t="s">
@@ -6713,7 +6713,7 @@
         <v>87</v>
       </c>
       <c r="O51" s="34" t="s">
-        <v>520</v>
+        <v>606</v>
       </c>
       <c r="P51" s="34" t="s">
         <v>87</v>
@@ -6725,7 +6725,7 @@
         <v>87</v>
       </c>
       <c r="S51" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T51" s="34"/>
       <c r="U51" s="35" t="s">
@@ -7209,7 +7209,7 @@
       <c r="T62" s="34"/>
       <c r="U62" s="35"/>
       <c r="V62" s="34" t="s">
-        <v>569</v>
+        <v>568</v>
       </c>
       <c r="W62" s="36" t="s">
         <v>67</v>
@@ -7235,13 +7235,13 @@
         <v>45532</v>
       </c>
       <c r="G63" s="33" t="s">
-        <v>574</v>
+        <v>573</v>
       </c>
       <c r="H63" s="33" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="I63" s="33" t="s">
-        <v>572</v>
+        <v>571</v>
       </c>
       <c r="J63" s="34" t="s">
         <v>87</v>
@@ -7255,7 +7255,7 @@
         <v>87</v>
       </c>
       <c r="O63" s="34" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="P63" s="34" t="s">
         <v>87</v>
@@ -7267,12 +7267,12 @@
         <v>87</v>
       </c>
       <c r="S63" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T63" s="34"/>
       <c r="U63" s="35"/>
       <c r="V63" s="34" t="s">
-        <v>571</v>
+        <v>570</v>
       </c>
       <c r="W63" s="36" t="s">
         <v>67</v>
@@ -7298,13 +7298,13 @@
         <v>45532</v>
       </c>
       <c r="G64" s="33" t="s">
+        <v>575</v>
+      </c>
+      <c r="H64" s="33" t="s">
         <v>576</v>
       </c>
-      <c r="H64" s="33" t="s">
+      <c r="I64" s="33" t="s">
         <v>577</v>
-      </c>
-      <c r="I64" s="33" t="s">
-        <v>578</v>
       </c>
       <c r="J64" s="34" t="s">
         <v>87</v>
@@ -7318,7 +7318,7 @@
         <v>87</v>
       </c>
       <c r="O64" s="34" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="P64" s="34" t="s">
         <v>87</v>
@@ -7330,12 +7330,12 @@
         <v>87</v>
       </c>
       <c r="S64" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T64" s="34"/>
       <c r="U64" s="35"/>
       <c r="V64" s="34" t="s">
-        <v>575</v>
+        <v>574</v>
       </c>
       <c r="W64" s="36" t="s">
         <v>67</v>
@@ -7361,13 +7361,13 @@
         <v>45533</v>
       </c>
       <c r="G65" s="33" t="s">
-        <v>582</v>
+        <v>581</v>
       </c>
       <c r="H65" s="33" t="s">
-        <v>581</v>
+        <v>580</v>
       </c>
       <c r="I65" s="33" t="s">
-        <v>580</v>
+        <v>579</v>
       </c>
       <c r="J65" s="34" t="s">
         <v>87</v>
@@ -7381,7 +7381,7 @@
         <v>87</v>
       </c>
       <c r="O65" s="34" t="s">
-        <v>570</v>
+        <v>569</v>
       </c>
       <c r="P65" s="34" t="s">
         <v>87</v>
@@ -7393,12 +7393,12 @@
         <v>87</v>
       </c>
       <c r="S65" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T65" s="34"/>
       <c r="U65" s="35"/>
       <c r="V65" s="34" t="s">
-        <v>579</v>
+        <v>578</v>
       </c>
       <c r="W65" s="36" t="s">
         <v>67</v>
@@ -7682,13 +7682,13 @@
         <v>45506</v>
       </c>
       <c r="G72" s="33" t="s">
+        <v>527</v>
+      </c>
+      <c r="H72" s="33" t="s">
         <v>528</v>
       </c>
-      <c r="H72" s="33" t="s">
+      <c r="I72" s="33" t="s">
         <v>529</v>
-      </c>
-      <c r="I72" s="33" t="s">
-        <v>530</v>
       </c>
       <c r="J72" s="34" t="s">
         <v>87</v>
@@ -7702,7 +7702,7 @@
         <v>87</v>
       </c>
       <c r="O72" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P72" s="34" t="s">
         <v>87</v>
@@ -7714,12 +7714,12 @@
         <v>87</v>
       </c>
       <c r="S72" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T72" s="34"/>
       <c r="U72" s="35"/>
       <c r="V72" s="34" t="s">
-        <v>527</v>
+        <v>526</v>
       </c>
       <c r="W72" s="36" t="s">
         <v>67</v>
@@ -7745,13 +7745,13 @@
         <v>45531</v>
       </c>
       <c r="G73" s="33" t="s">
+        <v>556</v>
+      </c>
+      <c r="H73" s="33" t="s">
         <v>557</v>
       </c>
-      <c r="H73" s="33" t="s">
+      <c r="I73" s="33" t="s">
         <v>558</v>
-      </c>
-      <c r="I73" s="33" t="s">
-        <v>559</v>
       </c>
       <c r="J73" s="34" t="s">
         <v>87</v>
@@ -7765,7 +7765,7 @@
         <v>87</v>
       </c>
       <c r="O73" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P73" s="34" t="s">
         <v>87</v>
@@ -7777,12 +7777,12 @@
         <v>87</v>
       </c>
       <c r="S73" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T73" s="34"/>
       <c r="U73" s="35"/>
       <c r="V73" s="34" t="s">
-        <v>556</v>
+        <v>555</v>
       </c>
       <c r="W73" s="36" t="s">
         <v>67</v>
@@ -8238,13 +8238,13 @@
         <v>45531</v>
       </c>
       <c r="G84" s="33" t="s">
+        <v>539</v>
+      </c>
+      <c r="H84" s="33" t="s">
         <v>540</v>
       </c>
-      <c r="H84" s="33" t="s">
+      <c r="I84" s="33" t="s">
         <v>541</v>
-      </c>
-      <c r="I84" s="33" t="s">
-        <v>542</v>
       </c>
       <c r="J84" s="34" t="s">
         <v>87</v>
@@ -8258,7 +8258,7 @@
         <v>87</v>
       </c>
       <c r="O84" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P84" s="34" t="s">
         <v>87</v>
@@ -8270,12 +8270,12 @@
         <v>87</v>
       </c>
       <c r="S84" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T84" s="34"/>
       <c r="U84" s="35"/>
       <c r="V84" s="34" t="s">
-        <v>539</v>
+        <v>538</v>
       </c>
       <c r="W84" s="36" t="s">
         <v>67</v>
@@ -8344,13 +8344,13 @@
         <v>45531</v>
       </c>
       <c r="G86" s="33" t="s">
+        <v>543</v>
+      </c>
+      <c r="H86" s="33" t="s">
         <v>544</v>
       </c>
-      <c r="H86" s="33" t="s">
+      <c r="I86" s="33" t="s">
         <v>545</v>
-      </c>
-      <c r="I86" s="33" t="s">
-        <v>546</v>
       </c>
       <c r="J86" s="34" t="s">
         <v>87</v>
@@ -8364,7 +8364,7 @@
         <v>87</v>
       </c>
       <c r="O86" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P86" s="34" t="s">
         <v>87</v>
@@ -8376,12 +8376,12 @@
         <v>87</v>
       </c>
       <c r="S86" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T86" s="34"/>
       <c r="U86" s="35"/>
       <c r="V86" s="64" t="s">
-        <v>543</v>
+        <v>542</v>
       </c>
       <c r="W86" s="36" t="s">
         <v>67</v>
@@ -8418,7 +8418,7 @@
       <c r="R87" s="34"/>
       <c r="S87" s="34"/>
       <c r="V87" s="65" t="s">
-        <v>547</v>
+        <v>546</v>
       </c>
       <c r="W87" s="36" t="s">
         <v>67</v>
@@ -8444,13 +8444,13 @@
         <v>45531</v>
       </c>
       <c r="G88" s="33" t="s">
+        <v>548</v>
+      </c>
+      <c r="H88" s="33" t="s">
+        <v>550</v>
+      </c>
+      <c r="I88" s="33" t="s">
         <v>549</v>
-      </c>
-      <c r="H88" s="33" t="s">
-        <v>551</v>
-      </c>
-      <c r="I88" s="33" t="s">
-        <v>550</v>
       </c>
       <c r="J88" s="34" t="s">
         <v>87</v>
@@ -8464,7 +8464,7 @@
         <v>87</v>
       </c>
       <c r="O88" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P88" s="34" t="s">
         <v>87</v>
@@ -8476,12 +8476,12 @@
         <v>87</v>
       </c>
       <c r="S88" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T88" s="34"/>
       <c r="U88" s="35"/>
       <c r="V88" s="34" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W88" s="36" t="s">
         <v>67</v>
@@ -8765,13 +8765,13 @@
         <v>45531</v>
       </c>
       <c r="G95" s="33" t="s">
+        <v>560</v>
+      </c>
+      <c r="H95" s="33" t="s">
         <v>561</v>
       </c>
-      <c r="H95" s="33" t="s">
+      <c r="I95" s="33" t="s">
         <v>562</v>
-      </c>
-      <c r="I95" s="33" t="s">
-        <v>563</v>
       </c>
       <c r="J95" s="34" t="s">
         <v>87</v>
@@ -8785,7 +8785,7 @@
         <v>87</v>
       </c>
       <c r="O95" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P95" s="34" t="s">
         <v>87</v>
@@ -8797,12 +8797,12 @@
         <v>87</v>
       </c>
       <c r="S95" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T95" s="34"/>
       <c r="U95" s="35"/>
       <c r="V95" s="34" t="s">
-        <v>560</v>
+        <v>559</v>
       </c>
       <c r="W95" s="36" t="s">
         <v>67</v>
@@ -11666,13 +11666,13 @@
         <v>45506</v>
       </c>
       <c r="G162" s="33" t="s">
+        <v>523</v>
+      </c>
+      <c r="H162" s="33" t="s">
+        <v>525</v>
+      </c>
+      <c r="I162" s="33" t="s">
         <v>524</v>
-      </c>
-      <c r="H162" s="33" t="s">
-        <v>526</v>
-      </c>
-      <c r="I162" s="33" t="s">
-        <v>525</v>
       </c>
       <c r="J162" s="34" t="s">
         <v>87</v>
@@ -11686,7 +11686,7 @@
         <v>87</v>
       </c>
       <c r="O162" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P162" s="34" t="s">
         <v>87</v>
@@ -11698,12 +11698,12 @@
         <v>87</v>
       </c>
       <c r="S162" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T162" s="34"/>
       <c r="U162" s="35"/>
       <c r="V162" s="34" t="s">
-        <v>523</v>
+        <v>522</v>
       </c>
       <c r="W162" s="36" t="s">
         <v>67</v>
@@ -11729,13 +11729,13 @@
         <v>45506</v>
       </c>
       <c r="G163" s="33" t="s">
+        <v>534</v>
+      </c>
+      <c r="H163" s="33" t="s">
+        <v>536</v>
+      </c>
+      <c r="I163" s="33" t="s">
         <v>535</v>
-      </c>
-      <c r="H163" s="33" t="s">
-        <v>537</v>
-      </c>
-      <c r="I163" s="33" t="s">
-        <v>536</v>
       </c>
       <c r="J163" s="34" t="s">
         <v>87</v>
@@ -11749,7 +11749,7 @@
         <v>87</v>
       </c>
       <c r="O163" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P163" s="34" t="s">
         <v>87</v>
@@ -11761,12 +11761,12 @@
         <v>87</v>
       </c>
       <c r="S163" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T163" s="34"/>
       <c r="U163" s="35"/>
       <c r="V163" s="34" t="s">
-        <v>534</v>
+        <v>533</v>
       </c>
       <c r="W163" s="36" t="s">
         <v>67</v>
@@ -11792,13 +11792,13 @@
         <v>45531</v>
       </c>
       <c r="G164" s="33" t="s">
+        <v>553</v>
+      </c>
+      <c r="H164" s="33" t="s">
+        <v>552</v>
+      </c>
+      <c r="I164" s="33" t="s">
         <v>554</v>
-      </c>
-      <c r="H164" s="33" t="s">
-        <v>553</v>
-      </c>
-      <c r="I164" s="33" t="s">
-        <v>555</v>
       </c>
       <c r="J164" s="34" t="s">
         <v>87</v>
@@ -11812,7 +11812,7 @@
         <v>87</v>
       </c>
       <c r="O164" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P164" s="34" t="s">
         <v>87</v>
@@ -11824,12 +11824,12 @@
         <v>87</v>
       </c>
       <c r="S164" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T164" s="34"/>
       <c r="U164" s="35"/>
       <c r="V164" s="34" t="s">
-        <v>548</v>
+        <v>547</v>
       </c>
       <c r="W164" s="36" t="s">
         <v>67</v>
@@ -11855,13 +11855,13 @@
         <v>45506</v>
       </c>
       <c r="G165" s="33" t="s">
+        <v>530</v>
+      </c>
+      <c r="H165" s="33" t="s">
         <v>531</v>
       </c>
-      <c r="H165" s="33" t="s">
+      <c r="I165" s="33" t="s">
         <v>532</v>
-      </c>
-      <c r="I165" s="33" t="s">
-        <v>533</v>
       </c>
       <c r="J165" s="34" t="s">
         <v>87</v>
@@ -11875,7 +11875,7 @@
         <v>87</v>
       </c>
       <c r="O165" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P165" s="34" t="s">
         <v>87</v>
@@ -11887,12 +11887,12 @@
         <v>87</v>
       </c>
       <c r="S165" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T165" s="34"/>
       <c r="U165" s="35"/>
       <c r="V165" s="34" t="s">
-        <v>552</v>
+        <v>551</v>
       </c>
       <c r="W165" s="36" t="s">
         <v>67</v>
@@ -11935,7 +11935,7 @@
       <c r="T166" s="34"/>
       <c r="U166" s="35"/>
       <c r="V166" s="34" t="s">
-        <v>538</v>
+        <v>537</v>
       </c>
       <c r="W166" s="36" t="s">
         <v>67</v>
@@ -12133,13 +12133,13 @@
         <v>45531</v>
       </c>
       <c r="G171" s="33" t="s">
-        <v>566</v>
+        <v>565</v>
       </c>
       <c r="H171" s="33" t="s">
-        <v>565</v>
+        <v>564</v>
       </c>
       <c r="I171" s="33" t="s">
-        <v>564</v>
+        <v>563</v>
       </c>
       <c r="J171" s="34" t="s">
         <v>87</v>
@@ -12153,7 +12153,7 @@
         <v>87</v>
       </c>
       <c r="O171" s="34" t="s">
-        <v>522</v>
+        <v>521</v>
       </c>
       <c r="P171" s="34" t="s">
         <v>87</v>
@@ -12165,12 +12165,12 @@
         <v>87</v>
       </c>
       <c r="S171" s="34" t="s">
-        <v>521</v>
+        <v>520</v>
       </c>
       <c r="T171" s="34"/>
       <c r="U171" s="35"/>
       <c r="V171" s="34" t="s">
-        <v>567</v>
+        <v>566</v>
       </c>
       <c r="W171" s="36" t="s">
         <v>67</v>
@@ -13013,13 +13013,13 @@
         <v>45544</v>
       </c>
       <c r="G191" s="33" t="s">
+        <v>585</v>
+      </c>
+      <c r="H191" s="33" t="s">
         <v>586</v>
       </c>
-      <c r="H191" s="33" t="s">
+      <c r="I191" s="33" t="s">
         <v>587</v>
-      </c>
-      <c r="I191" s="33" t="s">
-        <v>588</v>
       </c>
       <c r="J191" s="34" t="s">
         <v>87</v>
@@ -13060,13 +13060,13 @@
         <v>45544</v>
       </c>
       <c r="G192" s="33" t="s">
+        <v>603</v>
+      </c>
+      <c r="H192" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="H192" s="33" t="s">
+      <c r="I192" s="33" t="s">
         <v>605</v>
-      </c>
-      <c r="I192" s="33" t="s">
-        <v>606</v>
       </c>
       <c r="J192" s="34" t="s">
         <v>87</v>
@@ -13236,13 +13236,13 @@
         <v>45544</v>
       </c>
       <c r="G196" s="33" t="s">
+        <v>582</v>
+      </c>
+      <c r="H196" s="33" t="s">
         <v>583</v>
       </c>
-      <c r="H196" s="33" t="s">
+      <c r="I196" s="33" t="s">
         <v>584</v>
-      </c>
-      <c r="I196" s="33" t="s">
-        <v>585</v>
       </c>
       <c r="J196" s="34" t="s">
         <v>87</v>
@@ -14641,13 +14641,13 @@
         <v>45546</v>
       </c>
       <c r="G224" s="43" t="s">
+        <v>600</v>
+      </c>
+      <c r="H224" s="43" t="s">
         <v>601</v>
       </c>
-      <c r="H224" s="43" t="s">
+      <c r="I224" s="43" t="s">
         <v>602</v>
-      </c>
-      <c r="I224" s="43" t="s">
-        <v>603</v>
       </c>
       <c r="J224" s="44" t="s">
         <v>87</v>
@@ -21592,6 +21592,18 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A92AB09DCDF6014AA0D6826BF29E2C8E" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d4db60622090a1f8a8d506ac1d64a349">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="1e76d14e-d0ce-457c-8343-9b55836d9ead" xmlns:ns3="a56712a3-8dfd-4688-917a-22f0cf513b89" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0a3a9ed8bb952a3d76dd1e2fa3d624b9" ns2:_="" ns3:_="">
     <xsd:import namespace="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
@@ -21849,18 +21861,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="a56712a3-8dfd-4688-917a-22f0cf513b89" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <UserStoryALM xmlns="1e76d14e-d0ce-457c-8343-9b55836d9ead" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9413B232-C823-4C2A-B920-858F3EB4F277}">
   <ds:schemaRefs>
@@ -21870,6 +21870,23 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{188DA7F5-158B-4F2F-BE68-E8B30B468193}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21886,21 +21903,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6C4C806F-EC4E-4231-9462-6D32094C4603}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="a56712a3-8dfd-4688-917a-22f0cf513b89"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="1e76d14e-d0ce-457c-8343-9b55836d9ead"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>